<commit_message>
Added in customer File
</commit_message>
<xml_diff>
--- a/customer3.xlsx
+++ b/customer3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samdsouza/Documents/EatUp/EatUp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8717FF3B-9FFA-7C4B-85D8-5289CF242065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2654925-32AE-D74B-94C7-6972331B6365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="4480" windowWidth="26040" windowHeight="14940" xr2:uid="{CCE186C0-BCB3-264D-A68D-4D8B6DEDB4B5}"/>
+    <workbookView xWindow="11460" yWindow="2660" windowWidth="26040" windowHeight="14940" xr2:uid="{CCE186C0-BCB3-264D-A68D-4D8B6DEDB4B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Customer ID </t>
   </si>
@@ -55,12 +55,75 @@
   </si>
   <si>
     <t xml:space="preserve">Buck Guthrie </t>
+  </si>
+  <si>
+    <t>3/1/2020'</t>
+  </si>
+  <si>
+    <t>Deli Zone</t>
+  </si>
+  <si>
+    <t>3/3/2020'</t>
+  </si>
+  <si>
+    <t>Chipotle</t>
+  </si>
+  <si>
+    <t>3/10/2020'</t>
+  </si>
+  <si>
+    <t>Cheeba Hut</t>
+  </si>
+  <si>
+    <t>3/16/2020'</t>
+  </si>
+  <si>
+    <t>Flagstaff House</t>
+  </si>
+  <si>
+    <t>3/18/2020'</t>
+  </si>
+  <si>
+    <t>Moto Maki</t>
+  </si>
+  <si>
+    <t>3/20/2020'</t>
+  </si>
+  <si>
+    <t>Illegal Peet's</t>
+  </si>
+  <si>
+    <t>3/25/2020'</t>
+  </si>
+  <si>
+    <t>The Buff</t>
+  </si>
+  <si>
+    <t>3/30/2020'</t>
+  </si>
+  <si>
+    <t>Brasserie ten ten</t>
+  </si>
+  <si>
+    <t>4/1/2020'</t>
+  </si>
+  <si>
+    <t>Rio</t>
+  </si>
+  <si>
+    <t>4/2/2020'</t>
+  </si>
+  <si>
+    <t>The West End Tavern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -90,8 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,16 +470,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4655584-DE0E-CB4C-8C5F-A651E2FA4DDD}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -451,6 +517,146 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>11.75</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>178.67</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12.42</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10.51</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1">
+        <v>65.45</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1">
+        <v>80.650000000000006</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45.62</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>